<commit_message>
trying to fix spatcorr
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uark-my.sharepoint.com/personal/reetamm_uark_edu/Documents/documents/GitHub/nflows/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reetam/Documents/GitHub/nflows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{B71AA652-FC61-AE4F-B096-97E2CFA3D7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95A80146-1973-4B66-BBFF-7819980B308A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9263F21-C0E4-A343-8A14-496CEE46108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6902B945-74B7-E74A-A5D5-95B25980250C}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="16240" windowHeight="15720" activeTab="1" xr2:uid="{6902B945-74B7-E74A-A5D5-95B25980250C}"/>
   </bookViews>
   <sheets>
     <sheet name="application" sheetId="1" r:id="rId1"/>
-    <sheet name="sim" sheetId="2" r:id="rId2"/>
+    <sheet name="application_final" sheetId="3" r:id="rId2"/>
+    <sheet name="sim" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
   <si>
     <t>Wass</t>
   </si>
@@ -106,6 +107,15 @@
   </si>
   <si>
     <t>SPCDE_CCA</t>
+  </si>
+  <si>
+    <t>m=5</t>
+  </si>
+  <si>
+    <t>m=3</t>
+  </si>
+  <si>
+    <t>m=10</t>
   </si>
 </sst>
 </file>
@@ -164,10 +174,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,13 +514,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF67CFB-EEEC-374D-A628-6D98B015699A}">
   <dimension ref="A2:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="A2:M26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -542,8 +555,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -585,8 +598,8 @@
         <v>0.31580000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -626,8 +639,8 @@
         <v>1.0121</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -667,8 +680,8 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -708,8 +721,8 @@
         <v>3.95E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
@@ -751,8 +764,8 @@
         <v>0.11609999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -792,8 +805,8 @@
         <v>1.6704000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -833,8 +846,8 @@
         <v>0.11749999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -874,8 +887,8 @@
         <v>0.14760000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -915,7 +928,7 @@
         <v>9.0800000000000006E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -955,7 +968,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -965,7 +978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -975,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -985,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1025,8 +1038,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B17" t="s">
@@ -1068,8 +1081,8 @@
         <v>0.82599999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -1109,8 +1122,8 @@
         <v>1.0648</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -1150,8 +1163,8 @@
         <v>5.7700000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -1191,8 +1204,8 @@
         <v>2.3199999999999998E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B21" t="s">
@@ -1234,8 +1247,8 @@
         <v>0.24410000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>5</v>
       </c>
@@ -1275,8 +1288,8 @@
         <v>4.6100000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -1316,8 +1329,8 @@
         <v>8.48E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
       <c r="B24" t="s">
         <v>1</v>
       </c>
@@ -1357,8 +1370,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
       <c r="B25" t="s">
         <v>2</v>
       </c>
@@ -1398,7 +1411,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>6</v>
       </c>
@@ -1450,16 +1463,365 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89672D6A-14D1-F241-87EF-EAF3331B59EB}">
+  <dimension ref="A2:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="D3">
+        <v>0.30730000000000002</v>
+      </c>
+      <c r="E3">
+        <v>0.31950000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.32840000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.74909999999999999</v>
+      </c>
+      <c r="D4">
+        <v>0.94620000000000004</v>
+      </c>
+      <c r="E4">
+        <v>0.90810000000000002</v>
+      </c>
+      <c r="G4">
+        <v>0.91169999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>2.9100000000000001E-2</v>
+      </c>
+      <c r="G5">
+        <v>2.64E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0.54269999999999996</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.12559999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.14860000000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.14580000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1.927</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.276</v>
+      </c>
+      <c r="E7">
+        <v>1.2894000000000001</v>
+      </c>
+      <c r="G7">
+        <v>1.3023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0.1764</v>
+      </c>
+      <c r="D8">
+        <v>0.17080000000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.1036</v>
+      </c>
+      <c r="G8">
+        <v>0.1032</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>7.2400000000000006E-2</v>
+      </c>
+      <c r="D9">
+        <v>8.6800000000000002E-2</v>
+      </c>
+      <c r="E9">
+        <v>9.1300000000000006E-2</v>
+      </c>
+      <c r="G9">
+        <v>9.3399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.29749999999999999</v>
+      </c>
+      <c r="E10">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="G10">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1.3453999999999999</v>
+      </c>
+      <c r="D15">
+        <v>1.6735</v>
+      </c>
+      <c r="E15">
+        <v>0.90129999999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.89800000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>1.2756000000000001</v>
+      </c>
+      <c r="D16">
+        <v>1.7665999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.95640000000000003</v>
+      </c>
+      <c r="G16">
+        <v>1.0222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="D17">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="E17">
+        <v>2.9499999999999998E-2</v>
+      </c>
+      <c r="G17">
+        <v>2.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>0.85729999999999995</v>
+      </c>
+      <c r="D18">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="E18">
+        <v>0.26590000000000003</v>
+      </c>
+      <c r="G18">
+        <v>0.2331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>4.0202999999999998</v>
+      </c>
+      <c r="D19">
+        <v>4.66</v>
+      </c>
+      <c r="E19">
+        <v>4.1157000000000004</v>
+      </c>
+      <c r="G19">
+        <v>4.0395000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>8.3900000000000002E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.1656</v>
+      </c>
+      <c r="E20">
+        <v>8.4599999999999995E-2</v>
+      </c>
+      <c r="G20">
+        <v>8.5800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="D21">
+        <v>4.36E-2</v>
+      </c>
+      <c r="E21">
+        <v>4.58E-2</v>
+      </c>
+      <c r="G21">
+        <v>4.2900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>8.5500000000000007E-2</v>
+      </c>
+      <c r="D22">
+        <v>8.5500000000000007E-2</v>
+      </c>
+      <c r="E22">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G22">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE52D54D-64D7-4A21-8D0D-8FEC90DF1760}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1479,126 +1841,126 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>1.4936</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>1.4628000000000001</v>
       </c>
-      <c r="E2" s="4">
-        <v>0.2238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="E2" s="3">
+        <v>0.22070000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>1.9826999999999999</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>1.9484999999999999</v>
       </c>
-      <c r="E3" s="4">
-        <v>0.59930000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="E3" s="3">
+        <v>0.58260000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.52869999999999995</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>0.51870000000000005</v>
       </c>
-      <c r="E4" s="4">
-        <v>0.1285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="E4" s="3">
+        <v>0.1295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>2.1591999999999998</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>1.619</v>
       </c>
-      <c r="E5" s="4">
-        <v>0.46789999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="E5" s="3">
+        <v>0.46189999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>0.16700000000000001</v>
       </c>
-      <c r="E6" s="4">
-        <v>0.2452</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="E6" s="3">
+        <v>0.24970000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.26100000000000001</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0.20150000000000001</v>
       </c>
-      <c r="E7" s="4">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="E7" s="3">
+        <v>3.8899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0.45219999999999999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.48220000000000002</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>0.2258</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0.30159999999999998</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.37380000000000002</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated results and code for compiling results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reetam/Documents/GitHub/nflows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9263F21-C0E4-A343-8A14-496CEE46108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A870AB2-5327-FB41-9914-4A4FDBFDCE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="16240" windowHeight="15720" activeTab="1" xr2:uid="{6902B945-74B7-E74A-A5D5-95B25980250C}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" activeTab="1" xr2:uid="{6902B945-74B7-E74A-A5D5-95B25980250C}"/>
   </bookViews>
   <sheets>
-    <sheet name="application" sheetId="1" r:id="rId1"/>
+    <sheet name="application" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="application_final" sheetId="3" r:id="rId2"/>
     <sheet name="sim" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="30">
   <si>
     <t>Wass</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>m=10</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Full data</t>
+  </si>
+  <si>
+    <t>m=10,nolonlat</t>
   </si>
 </sst>
 </file>
@@ -150,12 +162,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -170,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -178,6 +196,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF67CFB-EEEC-374D-A628-6D98B015699A}">
   <dimension ref="A2:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1464,15 +1483,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89672D6A-14D1-F241-87EF-EAF3331B59EB}">
-  <dimension ref="A2:G22"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1483,16 +1507,16 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1506,13 +1530,16 @@
         <v>0.30730000000000002</v>
       </c>
       <c r="E3">
+        <v>0.30480000000000002</v>
+      </c>
+      <c r="F3">
         <v>0.31950000000000001</v>
       </c>
       <c r="G3">
         <v>0.32840000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>5</v>
@@ -1524,31 +1551,37 @@
         <v>0.94620000000000004</v>
       </c>
       <c r="E4">
+        <v>0.89449999999999996</v>
+      </c>
+      <c r="F4">
         <v>0.90810000000000002</v>
       </c>
       <c r="G4">
         <v>0.91169999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>3.3399999999999999E-2</v>
-      </c>
-      <c r="D5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="E5">
-        <v>2.9100000000000001E-2</v>
-      </c>
-      <c r="G5">
-        <v>2.64E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C5" s="5">
+        <v>4.1799999999999997E-2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3.7400000000000003E-2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4.8800000000000003E-2</v>
+      </c>
+      <c r="F5" s="5">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3.73E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1562,13 +1595,16 @@
         <v>0.12559999999999999</v>
       </c>
       <c r="E6">
+        <v>0.13969999999999999</v>
+      </c>
+      <c r="F6">
         <v>0.14860000000000001</v>
       </c>
       <c r="G6">
         <v>0.14580000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>5</v>
@@ -1580,13 +1616,16 @@
         <v>1.276</v>
       </c>
       <c r="E7">
+        <v>1.2889999999999999</v>
+      </c>
+      <c r="F7">
         <v>1.2894000000000001</v>
       </c>
       <c r="G7">
         <v>1.3023</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>4</v>
@@ -1598,31 +1637,37 @@
         <v>0.17080000000000001</v>
       </c>
       <c r="E8">
+        <v>0.10340000000000001</v>
+      </c>
+      <c r="F8">
         <v>0.1036</v>
       </c>
       <c r="G8">
         <v>0.1032</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C9">
-        <v>7.2400000000000006E-2</v>
-      </c>
-      <c r="D9">
-        <v>8.6800000000000002E-2</v>
-      </c>
-      <c r="E9">
-        <v>9.1300000000000006E-2</v>
-      </c>
-      <c r="G9">
-        <v>9.3399999999999997E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="5">
+        <v>9.6100000000000005E-2</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.11650000000000001</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.12740000000000001</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.1275</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.12839999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1635,11 +1680,14 @@
       <c r="E10">
         <v>8.0000000000000004E-4</v>
       </c>
+      <c r="F10">
+        <v>8.0000000000000004E-4</v>
+      </c>
       <c r="G10">
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1650,10 +1698,19 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1667,13 +1724,16 @@
         <v>1.6735</v>
       </c>
       <c r="E15">
+        <v>0.90720000000000001</v>
+      </c>
+      <c r="F15">
         <v>0.90129999999999999</v>
       </c>
       <c r="G15">
         <v>0.89800000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>5</v>
@@ -1685,31 +1745,37 @@
         <v>1.7665999999999999</v>
       </c>
       <c r="E16">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="F16">
         <v>0.95640000000000003</v>
       </c>
       <c r="G16">
         <v>1.0222</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C17">
-        <v>3.6600000000000001E-2</v>
-      </c>
-      <c r="D17">
-        <v>3.6600000000000001E-2</v>
-      </c>
-      <c r="E17">
-        <v>2.9499999999999998E-2</v>
-      </c>
-      <c r="G17">
-        <v>2.8500000000000001E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C17" s="5">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="D17" s="5">
+        <v>5.7099999999999998E-2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="F17" s="5">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3.5499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>8</v>
       </c>
@@ -1723,13 +1789,16 @@
         <v>0.47799999999999998</v>
       </c>
       <c r="E18">
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="F18">
         <v>0.26590000000000003</v>
       </c>
       <c r="G18">
         <v>0.2331</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>5</v>
@@ -1741,13 +1810,16 @@
         <v>4.66</v>
       </c>
       <c r="E19">
+        <v>3.8509000000000002</v>
+      </c>
+      <c r="F19">
         <v>4.1157000000000004</v>
       </c>
       <c r="G19">
         <v>4.0395000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>4</v>
@@ -1759,31 +1831,37 @@
         <v>0.1656</v>
       </c>
       <c r="E20">
+        <v>8.09E-2</v>
+      </c>
+      <c r="F20">
         <v>8.4599999999999995E-2</v>
       </c>
       <c r="G20">
         <v>8.5800000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C21">
-        <v>4.8500000000000001E-2</v>
-      </c>
-      <c r="D21">
-        <v>4.36E-2</v>
-      </c>
-      <c r="E21">
-        <v>4.58E-2</v>
-      </c>
-      <c r="G21">
-        <v>4.2900000000000001E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C21" s="5">
+        <v>9.0499999999999997E-2</v>
+      </c>
+      <c r="D21" s="5">
+        <v>9.9400000000000002E-2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="F21" s="5">
+        <v>7.9399999999999998E-2</v>
+      </c>
+      <c r="G21" s="5">
+        <v>7.9799999999999996E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>6</v>
       </c>
@@ -1796,16 +1874,374 @@
       <c r="E22">
         <v>5.0000000000000001E-4</v>
       </c>
+      <c r="F22">
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="G22">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0.12230000000000001</v>
+      </c>
+      <c r="D27">
+        <v>0.1057</v>
+      </c>
+      <c r="F27">
+        <v>0.1202</v>
+      </c>
+      <c r="G27">
+        <v>0.12809999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>0.28770000000000001</v>
+      </c>
+      <c r="D28">
+        <v>0.2329</v>
+      </c>
+      <c r="F28">
+        <v>0.34620000000000001</v>
+      </c>
+      <c r="G28">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="5">
+        <v>6.0199999999999997E-2</v>
+      </c>
+      <c r="D29" s="5">
+        <v>3.6700000000000003E-2</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="G29" s="5">
+        <v>2.3800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>0.4083</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.1537</v>
+      </c>
+      <c r="F30">
+        <v>7.4499999999999997E-2</v>
+      </c>
+      <c r="G30">
+        <v>7.7600000000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>0.54579999999999995</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.31809999999999999</v>
+      </c>
+      <c r="F31">
+        <v>0.74119999999999997</v>
+      </c>
+      <c r="G31">
+        <v>0.67479999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.18640000000000001</v>
+      </c>
+      <c r="F32">
+        <v>3.1099999999999999E-2</v>
+      </c>
+      <c r="G32">
+        <v>3.0200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="5">
+        <v>0.1439</v>
+      </c>
+      <c r="D33" s="5">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5">
+        <v>7.5800000000000006E-2</v>
+      </c>
+      <c r="G33" s="5">
+        <v>7.3400000000000007E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <v>0.30690000000000001</v>
+      </c>
+      <c r="D34">
+        <v>0.30690000000000001</v>
+      </c>
+      <c r="F34">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G34">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>1.2413000000000001</v>
+      </c>
+      <c r="D39">
+        <v>1.2391000000000001</v>
+      </c>
+      <c r="F39">
+        <v>0.125</v>
+      </c>
+      <c r="G39">
+        <v>0.1245</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>1.2202</v>
+      </c>
+      <c r="D40">
+        <v>1.1217999999999999</v>
+      </c>
+      <c r="F40">
+        <v>0.39129999999999998</v>
+      </c>
+      <c r="G40">
+        <v>0.42259999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="5">
+        <v>5.2299999999999999E-2</v>
+      </c>
+      <c r="D41" s="5">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5">
+        <v>2.06E-2</v>
+      </c>
+      <c r="G41" s="5">
+        <v>1.9800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>0.68510000000000004</v>
+      </c>
+      <c r="D42">
+        <v>0.54990000000000006</v>
+      </c>
+      <c r="F42">
+        <v>0.216</v>
+      </c>
+      <c r="G42">
+        <v>0.2301</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>2.0962000000000001</v>
+      </c>
+      <c r="D43">
+        <v>1.9834000000000001</v>
+      </c>
+      <c r="F43">
+        <v>1.9207000000000001</v>
+      </c>
+      <c r="G43">
+        <v>1.9759</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>0.1111</v>
+      </c>
+      <c r="D44">
+        <v>0.14269999999999999</v>
+      </c>
+      <c r="F44">
+        <v>2.07E-2</v>
+      </c>
+      <c r="G44">
+        <v>1.9900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="5">
+        <v>9.6799999999999997E-2</v>
+      </c>
+      <c r="D45" s="5">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="G45" s="5">
+        <v>4.2900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D46">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F46">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G46">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A45"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A27:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>